<commit_message>
Tambah referensi manual: 118976
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Referensi" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,23 +28,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -67,8 +57,8 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,8 +466,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>152</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>152</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -499,13 +491,17 @@
           <t>DINAS TENAGA KERJA DAN TRANSMIGRASI KABUPATEN OKU TIMUR</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>25</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -527,13 +523,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>2</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>115</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -555,13 +555,17 @@
           <t>SEKRETARIAT BAWASLU KABUPATEN OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>3</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>25</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -583,13 +587,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 3 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>4</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>25</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -611,13 +619,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>5</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>12</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -641,13 +653,17 @@
 BATURAJA KESDAM II/SWJ</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>6</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>66</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -669,13 +685,17 @@
           <t>BADAN NARKOTIKA NASIONAL KABUPATEN OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>7</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>56</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -697,13 +717,17 @@
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>8</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>25</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -725,13 +749,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>9</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>25</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -753,13 +781,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>10</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>115</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -781,13 +813,17 @@
           <t>SEKRETARIAT BAWASLU KABUPATEN OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>11</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>25</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -809,13 +845,17 @@
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>12</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>56</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -837,13 +877,17 @@
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>13</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>5</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -865,13 +909,17 @@
           <t>PENGADILAN NEGERI BATURAJA</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>14</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>25</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -893,13 +941,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>15</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>25</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -921,13 +973,17 @@
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>16</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>25</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -949,13 +1005,17 @@
           <t>MADRASAH ALIYAH NEGERI 2 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>17</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>137</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -977,13 +1037,17 @@
           <t>RUPBASAN KELAS II BATURAJA</t>
         </is>
       </c>
-      <c r="F19" t="n">
-        <v>18</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>25</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1005,13 +1069,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>19</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>25</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1033,13 +1101,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>20</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>137</v>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1061,13 +1133,17 @@
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F22" t="n">
-        <v>21</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>137</v>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1089,13 +1165,17 @@
           <t>LAPAS KELAS II B MUARA DUA</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>22</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>5</v>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1117,13 +1197,17 @@
           <t>PENGADILAN NEGERI BATURAJA</t>
         </is>
       </c>
-      <c r="F24" t="n">
-        <v>23</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1145,13 +1229,17 @@
           <t>LOKA LABORATORIUM KESEHATAN MASYARAKAT BATURAJA</t>
         </is>
       </c>
-      <c r="F25" t="n">
-        <v>24</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>6</v>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1173,13 +1261,17 @@
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F26" t="n">
-        <v>25</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>6</v>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1201,13 +1293,17 @@
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F27" t="n">
-        <v>26</v>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>25</v>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1229,13 +1325,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F28" t="n">
-        <v>27</v>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>25</v>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1257,13 +1357,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F29" t="n">
-        <v>28</v>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>25</v>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1285,13 +1389,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>29</v>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>6</v>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1313,13 +1421,17 @@
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>30</v>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>25</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1341,13 +1453,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F32" t="n">
-        <v>31</v>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>25</v>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1369,13 +1485,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 2 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F33" t="n">
-        <v>32</v>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>60</v>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1397,13 +1517,17 @@
           <t>POLRES OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F34" t="n">
-        <v>33</v>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>25</v>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1425,13 +1549,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 4 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>34</v>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>25</v>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1453,13 +1581,17 @@
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F36" t="n">
-        <v>35</v>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>76</v>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1481,13 +1613,17 @@
           <t>KPU KABUPATEN OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F37" t="n">
-        <v>36</v>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>25</v>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1509,13 +1645,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F38" t="n">
-        <v>37</v>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>25</v>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1537,13 +1677,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 2 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F39" t="n">
-        <v>38</v>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>76</v>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1565,13 +1709,17 @@
           <t>KPU KABUPATEN OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F40" t="n">
-        <v>39</v>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>12</v>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1593,13 +1741,17 @@
           <t>PUSLATPUR KODIKLATAD</t>
         </is>
       </c>
-      <c r="F41" t="n">
-        <v>40</v>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>56</v>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1621,13 +1773,17 @@
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU TIMUR PROV. SUMATRA SELATAN</t>
         </is>
       </c>
-      <c r="F42" t="n">
-        <v>41</v>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>25</v>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1649,13 +1805,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F43" t="n">
-        <v>42</v>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>25</v>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1677,13 +1837,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F44" t="n">
-        <v>43</v>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>25</v>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1705,13 +1869,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F45" t="n">
-        <v>44</v>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>25</v>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1733,13 +1901,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 3 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F46" t="n">
-        <v>45</v>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>25</v>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1761,13 +1933,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F47" t="n">
-        <v>46</v>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>76</v>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1789,13 +1965,17 @@
           <t>KPU KABUPATEN OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F48" t="n">
-        <v>47</v>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>5</v>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1817,13 +1997,17 @@
           <t>PENGADILAN AGAMA MUARADUA</t>
         </is>
       </c>
-      <c r="F49" t="n">
-        <v>48</v>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>60</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1845,13 +2029,17 @@
           <t>POLRES OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F50" t="n">
-        <v>49</v>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>25</v>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1873,13 +2061,17 @@
           <t>MADRASAH TSANAWIYAH NEGERI 4 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F51" t="n">
-        <v>50</v>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>25</v>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1901,13 +2093,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F52" t="n">
-        <v>51</v>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>137</v>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1929,13 +2125,17 @@
           <t>BAPAS KELAS II OKU INDUK</t>
         </is>
       </c>
-      <c r="F53" t="n">
-        <v>52</v>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>25</v>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1957,13 +2157,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F54" t="n">
-        <v>53</v>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>25</v>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1985,13 +2189,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F55" t="n">
-        <v>54</v>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>5</v>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2013,13 +2221,17 @@
           <t>PENGADILAN AGAMA MARTAPURA</t>
         </is>
       </c>
-      <c r="F56" t="n">
-        <v>55</v>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>5</v>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2041,13 +2253,17 @@
           <t>PENGADILAN AGAMA MUARADUA</t>
         </is>
       </c>
-      <c r="F57" t="n">
-        <v>56</v>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>5</v>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2069,13 +2285,17 @@
           <t>PENGADILAN AGAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F58" t="n">
-        <v>57</v>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>5</v>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2097,13 +2317,17 @@
           <t>PENGADILAN AGAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F59" t="n">
-        <v>58</v>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>5</v>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2125,13 +2349,17 @@
           <t>PENGADILAN AGAMA MARTAPURA</t>
         </is>
       </c>
-      <c r="F60" t="n">
-        <v>59</v>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>15</v>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -2153,13 +2381,17 @@
           <t>KANTOR PELAYANAN PAJAK PRATAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F61" t="n">
-        <v>60</v>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>54</v>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -2181,13 +2413,17 @@
           <t>BADAN PUSAT STATISTIK KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F62" t="n">
-        <v>61</v>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>25</v>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2209,13 +2445,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F63" t="n">
-        <v>62</v>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>25</v>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2237,13 +2477,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F64" t="n">
-        <v>63</v>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>15</v>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2265,13 +2509,17 @@
           <t>KANTOR PELAYANAN PERBENDAHARAAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F65" t="n">
-        <v>64</v>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>60</v>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2293,13 +2541,17 @@
           <t>POLRES OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F66" t="n">
-        <v>65</v>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>54</v>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2321,13 +2573,17 @@
           <t>BADAN PUSAT STATISTIK KAB. OKU SELATAN</t>
         </is>
       </c>
-      <c r="F67" t="n">
-        <v>66</v>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>54</v>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2349,13 +2605,17 @@
           <t>BADAN PUSAT STATISTIK KAB. OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F68" t="n">
-        <v>67</v>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>137</v>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -2377,13 +2637,17 @@
           <t>RUTAN KELAS II B BATURAJA</t>
         </is>
       </c>
-      <c r="F69" t="n">
-        <v>68</v>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>137</v>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -2405,13 +2669,17 @@
           <t>RUMAH TAHANAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F70" t="n">
-        <v>70</v>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>137</v>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -2433,13 +2701,17 @@
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F71" t="n">
-        <v>71</v>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>71</t>
+        </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>137</v>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2461,13 +2733,17 @@
           <t>BAPAS KELAS II OKU INDUK</t>
         </is>
       </c>
-      <c r="F72" t="n">
-        <v>72</v>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>137</v>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2489,13 +2765,17 @@
           <t>RUMAH PENYIMPANAN BENDA SITAAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F73" t="n">
-        <v>73</v>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>137</v>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2517,13 +2797,17 @@
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F74" t="n">
-        <v>74</v>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>74</t>
+        </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>24</v>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2545,13 +2829,17 @@
           <t>BALAI PENELITIAN DAN PENGEMBANGAN KESEHATAN BATURAJA</t>
         </is>
       </c>
-      <c r="F75" t="n">
-        <v>75</v>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>25</v>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2573,13 +2861,17 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F76" t="n">
-        <v>76</v>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>25</v>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2601,13 +2893,17 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F77" t="n">
-        <v>77</v>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>76</v>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2629,7 +2925,39 @@
           <t>KPU KABUPATEN PENUKAL ABAB LEMATANG ILIR</t>
         </is>
       </c>
-      <c r="F78" t="n">
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>015</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Kementerian Keuangan</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>118976</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>TESTT TESTTTT</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hapus referensi: 118976 - TEST
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,10 +491,8 @@
           <t>DINAS TENAGA KERJA DAN TRANSMIGRASI KABUPATEN OKU TIMUR</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -523,10 +521,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="F3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -555,10 +551,8 @@
           <t>SEKRETARIAT BAWASLU KABUPATEN OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="F4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -587,10 +581,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 3 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="F5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -619,10 +611,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="F6" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -653,10 +643,8 @@
 BATURAJA KESDAM II/SWJ</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="F7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -685,10 +673,8 @@
           <t>BADAN NARKOTIKA NASIONAL KABUPATEN OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="F8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -717,10 +703,8 @@
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="F9" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -749,10 +733,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="F10" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -781,10 +763,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="F11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -813,10 +793,8 @@
           <t>SEKRETARIAT BAWASLU KABUPATEN OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="F12" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="13">
@@ -845,10 +823,8 @@
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="F13" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -877,10 +853,8 @@
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="F14" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -909,10 +883,8 @@
           <t>PENGADILAN NEGERI BATURAJA</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="F15" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="16">
@@ -941,10 +913,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="F16" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="17">
@@ -973,10 +943,8 @@
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="F17" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
@@ -1005,10 +973,8 @@
           <t>MADRASAH ALIYAH NEGERI 2 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="F18" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1037,10 +1003,8 @@
           <t>RUPBASAN KELAS II BATURAJA</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="F19" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="20">
@@ -1069,10 +1033,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="F20" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -1101,10 +1063,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="F21" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -1133,10 +1093,8 @@
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="F22" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="23">
@@ -1165,10 +1123,8 @@
           <t>LAPAS KELAS II B MUARA DUA</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="F23" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -1197,10 +1153,8 @@
           <t>PENGADILAN NEGERI BATURAJA</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="F24" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -1229,10 +1183,8 @@
           <t>LOKA LABORATORIUM KESEHATAN MASYARAKAT BATURAJA</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+      <c r="F25" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="26">
@@ -1261,10 +1213,8 @@
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="F26" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="27">
@@ -1293,10 +1243,8 @@
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="F27" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="28">
@@ -1325,10 +1273,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="F28" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="29">
@@ -1357,10 +1303,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="F29" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="30">
@@ -1389,10 +1333,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="F30" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="31">
@@ -1421,10 +1363,8 @@
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="F31" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="32">
@@ -1453,10 +1393,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+      <c r="F32" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="33">
@@ -1485,10 +1423,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 2 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
+      <c r="F33" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="34">
@@ -1517,10 +1453,8 @@
           <t>POLRES OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+      <c r="F34" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="35">
@@ -1549,10 +1483,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 4 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+      <c r="F35" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="36">
@@ -1581,10 +1513,8 @@
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="F36" t="n">
+        <v>35</v>
       </c>
     </row>
     <row r="37">
@@ -1613,10 +1543,8 @@
           <t>KPU KABUPATEN OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+      <c r="F37" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="38">
@@ -1645,10 +1573,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+      <c r="F38" t="n">
+        <v>37</v>
       </c>
     </row>
     <row r="39">
@@ -1677,10 +1603,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 2 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+      <c r="F39" t="n">
+        <v>38</v>
       </c>
     </row>
     <row r="40">
@@ -1709,10 +1633,8 @@
           <t>KPU KABUPATEN OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="F40" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="41">
@@ -1741,10 +1663,8 @@
           <t>PUSLATPUR KODIKLATAD</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="F41" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="42">
@@ -1773,10 +1693,8 @@
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU TIMUR PROV. SUMATRA SELATAN</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+      <c r="F42" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="43">
@@ -1805,10 +1723,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>42</t>
-        </is>
+      <c r="F43" t="n">
+        <v>42</v>
       </c>
     </row>
     <row r="44">
@@ -1837,10 +1753,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+      <c r="F44" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="45">
@@ -1869,10 +1783,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+      <c r="F45" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="46">
@@ -1901,10 +1813,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 3 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="F46" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="47">
@@ -1933,10 +1843,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>46</t>
-        </is>
+      <c r="F47" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="48">
@@ -1965,10 +1873,8 @@
           <t>KPU KABUPATEN OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+      <c r="F48" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="49">
@@ -1997,10 +1903,8 @@
           <t>PENGADILAN AGAMA MUARADUA</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+      <c r="F49" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="50">
@@ -2029,10 +1933,8 @@
           <t>POLRES OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+      <c r="F50" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="51">
@@ -2061,10 +1963,8 @@
           <t>MADRASAH TSANAWIYAH NEGERI 4 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="F51" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="52">
@@ -2093,10 +1993,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>51</t>
-        </is>
+      <c r="F52" t="n">
+        <v>51</v>
       </c>
     </row>
     <row r="53">
@@ -2125,10 +2023,8 @@
           <t>BAPAS KELAS II OKU INDUK</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>52</t>
-        </is>
+      <c r="F53" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="54">
@@ -2157,10 +2053,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>53</t>
-        </is>
+      <c r="F54" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="55">
@@ -2189,10 +2083,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
+      <c r="F55" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="56">
@@ -2221,10 +2113,8 @@
           <t>PENGADILAN AGAMA MARTAPURA</t>
         </is>
       </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
+      <c r="F56" t="n">
+        <v>55</v>
       </c>
     </row>
     <row r="57">
@@ -2253,10 +2143,8 @@
           <t>PENGADILAN AGAMA MUARADUA</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>56</t>
-        </is>
+      <c r="F57" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="58">
@@ -2285,10 +2173,8 @@
           <t>PENGADILAN AGAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+      <c r="F58" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="59">
@@ -2317,10 +2203,8 @@
           <t>PENGADILAN AGAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="F59" t="n">
+        <v>58</v>
       </c>
     </row>
     <row r="60">
@@ -2349,10 +2233,8 @@
           <t>PENGADILAN AGAMA MARTAPURA</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="F60" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="61">
@@ -2381,10 +2263,8 @@
           <t>KANTOR PELAYANAN PAJAK PRATAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="F61" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="62">
@@ -2413,10 +2293,8 @@
           <t>BADAN PUSAT STATISTIK KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
+      <c r="F62" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="63">
@@ -2445,10 +2323,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+      <c r="F63" t="n">
+        <v>62</v>
       </c>
     </row>
     <row r="64">
@@ -2477,10 +2353,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
+      <c r="F64" t="n">
+        <v>63</v>
       </c>
     </row>
     <row r="65">
@@ -2509,10 +2383,8 @@
           <t>KANTOR PELAYANAN PERBENDAHARAAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>64</t>
-        </is>
+      <c r="F65" t="n">
+        <v>64</v>
       </c>
     </row>
     <row r="66">
@@ -2541,10 +2413,8 @@
           <t>POLRES OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+      <c r="F66" t="n">
+        <v>65</v>
       </c>
     </row>
     <row r="67">
@@ -2573,10 +2443,8 @@
           <t>BADAN PUSAT STATISTIK KAB. OKU SELATAN</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+      <c r="F67" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="68">
@@ -2605,10 +2473,8 @@
           <t>BADAN PUSAT STATISTIK KAB. OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>67</t>
-        </is>
+      <c r="F68" t="n">
+        <v>67</v>
       </c>
     </row>
     <row r="69">
@@ -2637,10 +2503,8 @@
           <t>RUTAN KELAS II B BATURAJA</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+      <c r="F69" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="70">
@@ -2669,10 +2533,8 @@
           <t>RUMAH TAHANAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+      <c r="F70" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="71">
@@ -2701,10 +2563,8 @@
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>71</t>
-        </is>
+      <c r="F71" t="n">
+        <v>70</v>
       </c>
     </row>
     <row r="72">
@@ -2733,10 +2593,8 @@
           <t>BAPAS KELAS II OKU INDUK</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>72</t>
-        </is>
+      <c r="F72" t="n">
+        <v>71</v>
       </c>
     </row>
     <row r="73">
@@ -2765,10 +2623,8 @@
           <t>RUMAH PENYIMPANAN BENDA SITAAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>73</t>
-        </is>
+      <c r="F73" t="n">
+        <v>72</v>
       </c>
     </row>
     <row r="74">
@@ -2797,10 +2653,8 @@
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>74</t>
-        </is>
+      <c r="F74" t="n">
+        <v>73</v>
       </c>
     </row>
     <row r="75">
@@ -2829,10 +2683,8 @@
           <t>BALAI PENELITIAN DAN PENGEMBANGAN KESEHATAN BATURAJA</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>75</t>
-        </is>
+      <c r="F75" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="76">
@@ -2861,10 +2713,8 @@
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>76</t>
-        </is>
+      <c r="F76" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="77">
@@ -2893,10 +2743,8 @@
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+      <c r="F77" t="n">
+        <v>76</v>
       </c>
     </row>
     <row r="78">
@@ -2925,40 +2773,8 @@
           <t>KPU KABUPATEN PENUKAL ABAB LEMATANG ILIR</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>78</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>015</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Kementerian Keuangan</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>118976</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>TESTT TESTTTT</t>
-        </is>
-      </c>
-      <c r="F79" t="n">
-        <v>78</v>
+      <c r="F78" t="n">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tambah referensi manual: 112233
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2777,6 +2777,36 @@
         <v>77</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>015</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Kementerian Keuangan</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>112233</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>TESTT</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>TESTT TESTTTTTTTTTT</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Hapus referensi: 112233 - TESTT
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2777,36 +2777,6 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>015</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Kementerian Keuangan</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>112233</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>TESTT</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>TESTT TESTTTTTTTTTT</t>
-        </is>
-      </c>
-      <c r="F79" t="n">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tambah referensi manual: 111222
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,2345 +436,2375 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Kode BA</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>K/L</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Kode Satker</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Uraian Satker-SINGKAT</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Uraian Satker-LENGKAP</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>152</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>TRANSMIGRASI</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>691653</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>DISNAKERTRANS OKUT</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>DINAS TENAGA KERJA DAN TRANSMIGRASI KABUPATEN OKU TIMUR</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>418461</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>KEMENAG OKU</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>115</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>BAWASLU</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>419006</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>BAWASLU OKU</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>SEKRETARIAT BAWASLU KABUPATEN OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>574370</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>MTSN 3 OKUS</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 3 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>666502</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>KEMENHAN</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>344894</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>RUMKIT NOESMIR</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>RUMKIT TK. III
 02.06.02 DR. NOESMIR
 BATURAJA KESDAM II/SWJ</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>66</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>BNN</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>111079</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>BNN OKUT</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>BADAN NARKOTIKA NASIONAL KABUPATEN OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F8" t="n">
-        <v>7</v>
-      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>ATR/BPN</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>431142</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>BPN OKU</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F9" t="n">
-        <v>8</v>
-      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>418459</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>KEMENAG OKU</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F10" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>418457</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>KEMENAG OKU</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F11" t="n">
-        <v>10</v>
-      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>115</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>BAWASLU</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>686503</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>BAWASLU OKUS</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>SEKRETARIAT BAWASLU KABUPATEN OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F12" t="n">
-        <v>11</v>
-      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>424245</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>MAN 1 OKU</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F13" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>ATR/BPN</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>670561</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>BPN OKUS</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F14" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>099228</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>PN BATURAJA</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>PENGADILAN NEGERI BATURAJA</t>
         </is>
       </c>
-      <c r="F15" t="n">
-        <v>14</v>
-      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A16" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>666503</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F16" t="n">
-        <v>15</v>
-      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A17" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>426066</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>MAN 1 OKUT</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F17" t="n">
-        <v>16</v>
-      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A18" t="n">
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>597558</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>MAN 2 OKUS</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>MADRASAH ALIYAH NEGERI 2 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F18" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>692725</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>RUPBASAN BATURAJA</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>RUPBASAN KELAS II BATURAJA</t>
         </is>
       </c>
-      <c r="F19" t="n">
-        <v>18</v>
-      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A20" t="n">
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>426050</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>MTSN 1 OKU</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F20" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A21" t="n">
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>666507</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F21" t="n">
-        <v>20</v>
-      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>692340</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>LAPAS MARTAPURA</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F22" t="n">
-        <v>21</v>
-      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>692334</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>LAPAS MUARA DUA</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>LAPAS KELAS II B MUARA DUA</t>
         </is>
       </c>
-      <c r="F23" t="n">
-        <v>22</v>
-      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>098963</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>PN BATURAJA</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>PENGADILAN NEGERI BATURAJA</t>
         </is>
       </c>
-      <c r="F24" t="n">
-        <v>23</v>
-      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>KEMENKES</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>690801</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>LOKA LABKESMAS</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>LOKA LABORATORIUM KESEHATAN MASYARAKAT BATURAJA</t>
         </is>
       </c>
-      <c r="F25" t="n">
-        <v>24</v>
-      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>KEJAKSAAN</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>007208</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>KEJARI OKUS</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F26" t="n">
-        <v>25</v>
-      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>KEJAKSAAN</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>007190</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>KEJARI OKUT</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F27" t="n">
-        <v>26</v>
-      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A28" t="n">
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>440502</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>KEMENAG OKUS</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F28" t="n">
-        <v>27</v>
-      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A29" t="n">
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>418458</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>KEMENAG OKU</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F29" t="n">
-        <v>28</v>
-      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A30" t="n">
+        <v>29</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>424967</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>MTSN 1 OKUT</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F30" t="n">
-        <v>29</v>
-      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>KEJAKSAAN</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>007130</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>KEJARI  OKU</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>KEJAKSAAN NEGERI OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F31" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A32" t="n">
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>553792</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>MTSN 1 OKUS</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 1 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F32" t="n">
-        <v>31</v>
-      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A33" t="n">
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>418462</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>MTSN 2 OKUS</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 2 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F33" t="n">
-        <v>32</v>
-      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>POLRI</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>665292</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>POLRES OKUT</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>POLRES OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F34" t="n">
-        <v>33</v>
-      </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A35" t="n">
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>661192</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>MTSN 4 OKUS</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 4 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F35" t="n">
-        <v>34</v>
-      </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A36" t="n">
+        <v>35</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>662127</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>MAN 1 OKUS</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>MADRASAH ALIYAH NEGERI 1 OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F36" t="n">
-        <v>35</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>76</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>KPU</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>656560</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>KPU OKUT</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>KPU KABUPATEN OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F37" t="n">
-        <v>36</v>
-      </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A38" t="n">
+        <v>37</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t>666505</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F38" t="n">
-        <v>37</v>
-      </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A39" t="n">
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>418471</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>MTSN 2 OKUT</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 2 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F39" t="n">
-        <v>38</v>
-      </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>76</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>KPU</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>656574</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>KPU OKUS</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>KPU KABUPATEN OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F40" t="n">
-        <v>39</v>
-      </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>KEMENHAN</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>685001</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>PUSLATPUR AD</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>PUSLATPUR KODIKLATAD</t>
         </is>
       </c>
-      <c r="F41" t="n">
-        <v>40</v>
-      </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>56</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>ATR/BPN</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>669055</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>BPN OKUT</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>KANTOR PERTANAHAN KAB. OGAN KOMERING ULU TIMUR PROV. SUMATRA SELATAN</t>
         </is>
       </c>
-      <c r="F42" t="n">
-        <v>41</v>
-      </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A43" t="n">
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>418456</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>KEMENAG OKU</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F43" t="n">
-        <v>42</v>
-      </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A44" t="n">
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>111071</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F44" t="n">
-        <v>43</v>
-      </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A45" t="n">
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>666501</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F45" t="n">
-        <v>44</v>
-      </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A46" t="n">
+        <v>45</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>553099</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>MTSN 3 OKUT</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 3 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F46" t="n">
-        <v>45</v>
-      </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A47" t="n">
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
           <t>440504</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>KEMENAG OKUS</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F47" t="n">
-        <v>46</v>
-      </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
         <is>
           <t>76</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>KPU</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>656553</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>KPU OKU</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>KPU KABUPATEN OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F48" t="n">
-        <v>47</v>
-      </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>403410</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>PA  MUARADUA</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>PENGADILAN AGAMA MUARADUA</t>
         </is>
       </c>
-      <c r="F49" t="n">
-        <v>48</v>
-      </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>POLRI</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>641681</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>POLRES OKU</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>POLRES OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F50" t="n">
-        <v>49</v>
-      </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A51" t="n">
+        <v>50</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>597480</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>MTSN 4 OKUT</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>MADRASAH TSANAWIYAH NEGERI 4 OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F51" t="n">
-        <v>50</v>
-      </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A52" t="n">
+        <v>51</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>666504</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F52" t="n">
-        <v>51</v>
-      </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>692625</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>BAPAS OKU INDUK</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>BAPAS KELAS II OKU INDUK</t>
         </is>
       </c>
-      <c r="F53" t="n">
-        <v>52</v>
-      </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A54" t="n">
+        <v>53</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
           <t>440503</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>KEMENAG OKUS</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F54" t="n">
-        <v>53</v>
-      </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A55" t="n">
+        <v>54</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
           <t>440506</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>KEMENAG OKUS</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F55" t="n">
-        <v>54</v>
-      </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>401944</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>PA MARTAPURA</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="F56" t="inlineStr">
         <is>
           <t>PENGADILAN AGAMA MARTAPURA</t>
         </is>
       </c>
-      <c r="F56" t="n">
-        <v>55</v>
-      </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>401945</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>PA MUARADUA</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>PENGADILAN AGAMA MUARADUA</t>
         </is>
       </c>
-      <c r="F57" t="n">
-        <v>56</v>
-      </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>402267</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>PA BATURAJA</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t>PENGADILAN AGAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F58" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
+      <c r="C59" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>402268</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>PA BATURAJA</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="F59" t="inlineStr">
         <is>
           <t>PENGADILAN AGAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F59" t="n">
-        <v>58</v>
-      </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="C60" t="inlineStr">
         <is>
           <t>MA</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>403409</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>PA MARTAPURA</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>PENGADILAN AGAMA MARTAPURA</t>
         </is>
       </c>
-      <c r="F60" t="n">
-        <v>59</v>
-      </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
+      <c r="C61" t="inlineStr">
         <is>
           <t>KEMENKEU</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>410574</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>KPP BATURAJA</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>KANTOR PELAYANAN PAJAK PRATAMA BATURAJA</t>
         </is>
       </c>
-      <c r="F61" t="n">
-        <v>60</v>
-      </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
+      <c r="C62" t="inlineStr">
         <is>
           <t>BPS</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>428258</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>BPS OKU</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="F62" t="inlineStr">
         <is>
           <t>BADAN PUSAT STATISTIK KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F62" t="n">
-        <v>61</v>
-      </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A63" t="n">
+        <v>62</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
           <t>440505</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>KEMENAG OKUS</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="F63" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F63" t="n">
-        <v>62</v>
-      </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A64" t="n">
+        <v>63</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
           <t>440507</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>KEMENAG OKUS</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="F64" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F64" t="n">
-        <v>63</v>
-      </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="C65" t="inlineStr">
         <is>
           <t>KEMENKEU</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>527975</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>KPPN BATURAJA</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="F65" t="inlineStr">
         <is>
           <t>KANTOR PELAYANAN PERBENDAHARAAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F65" t="n">
-        <v>64</v>
-      </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
         <is>
           <t>60</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>POLRI</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>665307</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>POLRES OKUS</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>POLRES OGAN KOMERING ULU SELATAN</t>
         </is>
       </c>
-      <c r="F66" t="n">
-        <v>65</v>
-      </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
+      <c r="C67" t="inlineStr">
         <is>
           <t>BPS</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>667215</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>BPS OKUS</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="F67" t="inlineStr">
         <is>
           <t>BADAN PUSAT STATISTIK KAB. OKU SELATAN</t>
         </is>
       </c>
-      <c r="F67" t="n">
-        <v>66</v>
-      </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>54</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>BPS</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>668529</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>BPS OKUT</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="F68" t="inlineStr">
         <is>
           <t>BADAN PUSAT STATISTIK KAB. OGAN KOMERING ULU TIMUR</t>
         </is>
       </c>
-      <c r="F68" t="n">
-        <v>67</v>
-      </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>692339</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>RUTAN BATURAJA</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="F69" t="inlineStr">
         <is>
           <t>RUTAN KELAS II B BATURAJA</t>
         </is>
       </c>
-      <c r="F69" t="n">
-        <v>68</v>
-      </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>406472</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>RUTAN BATURAJA</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="F70" t="inlineStr">
         <is>
           <t>RUMAH TAHANAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F70" t="n">
-        <v>69</v>
-      </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>406426</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>LAPAS MARTAPURA</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="F71" t="inlineStr">
         <is>
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F71" t="n">
-        <v>70</v>
-      </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>632013</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>BAPAS OKU INDUK</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t>BAPAS KELAS II OKU INDUK</t>
         </is>
       </c>
-      <c r="F72" t="n">
-        <v>71</v>
-      </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>653271</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>RUPBASAN BATURAJA</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="F73" t="inlineStr">
         <is>
           <t>RUMAH PENYIMPANAN BENDA SITAAN NEGARA BATURAJA</t>
         </is>
       </c>
-      <c r="F73" t="n">
-        <v>72</v>
-      </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
         <is>
           <t>137</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>IMIGRASIPAS</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>406488</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>LAPAS MARTAPURA</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="F74" t="inlineStr">
         <is>
           <t>LAPAS KELAS II B MARTAPURA</t>
         </is>
       </c>
-      <c r="F74" t="n">
-        <v>73</v>
-      </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>KEMENKES</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>653530</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>LOKA LABKESMAS</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="F75" t="inlineStr">
         <is>
           <t>BALAI PENELITIAN DAN PENGEMBANGAN KESEHATAN BATURAJA</t>
         </is>
       </c>
-      <c r="F75" t="n">
-        <v>74</v>
-      </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A76" t="n">
+        <v>75</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
           <t>666506</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>KEMENAG OKUT</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="F76" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA OKU TIMUR</t>
         </is>
       </c>
-      <c r="F76" t="n">
-        <v>75</v>
-      </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="A77" t="n">
+        <v>76</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>KEMENAG</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t>KEMENAG</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
           <t>418460</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>KEMENAG OKU</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="F77" t="inlineStr">
         <is>
           <t>KANTOR KEMENTERIAN AGAMA KAB. OGAN KOMERING ULU</t>
         </is>
       </c>
-      <c r="F77" t="n">
-        <v>76</v>
-      </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
         <is>
           <t>76</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="C78" t="inlineStr">
         <is>
           <t>KPU</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>111804</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>KPU PALI</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="F78" t="inlineStr">
         <is>
           <t>KPU KABUPATEN PENUKAL ABAB LEMATANG ILIR</t>
         </is>
       </c>
-      <c r="F78" t="n">
-        <v>77</v>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>015</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Kementerian Keuangan</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>111222</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>TESTTTTTTTTTT</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hapus referensi: 111222 - TEST
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2777,36 +2777,6 @@
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>78</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>015</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Kementerian Keuangan</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>111222</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>TESTTTTTTTTTT</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tambah referensi manual: 123123
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2777,6 +2777,36 @@
         </is>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>015</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Kementerian Keuangan</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>123123</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>TESTTTTTTTT AJAAAAAAAAAA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Hapus referensi: 123123 - TEST
</commit_message>
<xml_diff>
--- a/templates/Template_Data_Referensi.xlsx
+++ b/templates/Template_Data_Referensi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2777,36 +2777,6 @@
         </is>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>78</v>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>015</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Kementerian Keuangan</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>123123</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>TESTTTTTTTT AJAAAAAAAAAA</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>